<commit_message>
[Modify]30392 30395 30710 ~ 30760 50010
</commit_message>
<xml_diff>
--- a/PhoenixCI/Excel_Template/30392.xlsx
+++ b/PhoenixCI/Excel_Template/30392.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Source\Repos\buckblader\RekindlePhoenixCI\PhoenixCI\Excel_Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\PhoenixCI_GitHub\RekindlePhoenixCI\PhoenixCI\Excel_Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB36CA20-B402-45FE-94A7-ED2319A4E206}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195B1E48-105D-44DC-8A15-51C7FCCF6F3B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="882" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="882" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="30392_1(TJF)" sheetId="1" r:id="rId1"/>
@@ -51,12 +51,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>maewu</author>
   </authors>
   <commentList>
-    <comment ref="G4" authorId="0" shapeId="0">
+    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -90,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="0" shapeId="0">
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -130,12 +130,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>maewu</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -174,12 +174,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>maewu</author>
   </authors>
   <commentList>
-    <comment ref="G4" authorId="0" shapeId="0">
+    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -218,12 +218,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>maewu</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0B00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -262,12 +262,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>maewu</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0C00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -306,12 +306,12 @@
 </file>
 
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>maewu</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0D00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -350,12 +350,12 @@
 </file>
 
 <file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>maewu</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0E00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -394,12 +394,12 @@
 </file>
 
 <file path=xl/comments8.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>maewu</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0F00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -438,12 +438,12 @@
 </file>
 
 <file path=xl/comments9.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>maewu</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1546,17 +1546,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
     <numFmt numFmtId="176" formatCode="#,##0_);[Red]\(#,##0\)"/>
     <numFmt numFmtId="177" formatCode="#,##0_ "/>
     <numFmt numFmtId="178" formatCode="0.00_ "/>
     <numFmt numFmtId="179" formatCode="0.0000_ ;[Red]\-0.0000\ "/>
     <numFmt numFmtId="180" formatCode="0.00_ ;[Red]\-0.00\ "/>
-    <numFmt numFmtId="182" formatCode="0_ ;[Red]\-0\ "/>
-    <numFmt numFmtId="183" formatCode="0_ "/>
+    <numFmt numFmtId="181" formatCode="0_ ;[Red]\-0\ "/>
+    <numFmt numFmtId="182" formatCode="0_ "/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="新細明體"/>
@@ -1649,13 +1649,6 @@
       <color indexed="60"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="新細明體"/>
-      <family val="1"/>
-      <charset val="136"/>
     </font>
     <font>
       <sz val="9"/>
@@ -2503,10 +2496,10 @@
     <xf numFmtId="176" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="18" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="17" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="176" fontId="18" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="17" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="180" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2550,16 +2543,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="18" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="179" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2568,73 +2561,73 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="179" fontId="18" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="17" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="179" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="179" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="18" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="177" fontId="17" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="177" fontId="18" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="17" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="176" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="179" fontId="7" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="18" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2695,7 +2688,7 @@
     <xf numFmtId="177" fontId="10" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="3" borderId="12" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2716,42 +2709,51 @@
     <xf numFmtId="178" fontId="13" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="17" fillId="3" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="179" fontId="18" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="17" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="180" fontId="4" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="177" fontId="18" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="17" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="180" fontId="4" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="3" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="17" fillId="3" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="179" fontId="18" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="17" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="180" fontId="4" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="177" fontId="18" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="17" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2760,55 +2762,52 @@
     <xf numFmtId="0" fontId="28" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="27" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="27" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="182" fontId="28" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2817,31 +2816,25 @@
     <xf numFmtId="182" fontId="28" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="29" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="183" fontId="29" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="28" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="29" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="182" fontId="28" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="183" fontId="29" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="182" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="182" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2863,28 +2856,28 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2926,7 +2919,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2974,43 +2967,43 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3025,28 +3018,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6801,7 +6794,7 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="91" workbookViewId="0"/>
@@ -6814,10 +6807,10 @@
 </file>
 
 <file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -6830,7 +6823,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9191625" cy="5610225"/>
+    <xdr:ext cx="9200522" cy="5610330"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="圖表 1">
@@ -6949,7 +6942,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9210675" cy="5619750"/>
+    <xdr:ext cx="9222441" cy="5625353"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="圖表 1">
@@ -7411,7 +7404,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
@@ -7421,7 +7414,7 @@
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="12" style="17" customWidth="1"/>
@@ -7434,7 +7427,7 @@
     <col min="9" max="9" width="12" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="141" t="s">
         <v>16</v>
       </c>
@@ -7449,7 +7442,7 @@
       </c>
       <c r="J1" s="140"/>
     </row>
-    <row r="2" spans="1:10" ht="28.5">
+    <row r="2" spans="1:10" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -7481,7 +7474,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="24"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -7493,7 +7486,7 @@
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="24"/>
       <c r="B4" s="23"/>
       <c r="C4" s="26">
@@ -7517,7 +7510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="24"/>
       <c r="B5" s="23"/>
       <c r="C5" s="26">
@@ -7541,7 +7534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="23"/>
       <c r="C6" s="26">
@@ -7565,7 +7558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="24"/>
       <c r="B7" s="23"/>
       <c r="C7" s="26">
@@ -7589,7 +7582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
       <c r="B8" s="23"/>
       <c r="C8" s="26">
@@ -7613,7 +7606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="23"/>
       <c r="C9" s="26">
@@ -7637,7 +7630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="23"/>
       <c r="C10" s="26">
@@ -7661,7 +7654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="23"/>
       <c r="C11" s="26">
@@ -7685,7 +7678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="23"/>
       <c r="C12" s="26">
@@ -7709,7 +7702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="24"/>
       <c r="B13" s="23"/>
       <c r="C13" s="26">
@@ -7733,7 +7726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
       <c r="B14" s="23"/>
       <c r="C14" s="26">
@@ -7757,7 +7750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="24"/>
       <c r="B15" s="23"/>
       <c r="C15" s="26">
@@ -7781,7 +7774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
       <c r="B16" s="23"/>
       <c r="C16" s="26">
@@ -7805,7 +7798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
       <c r="B17" s="23"/>
       <c r="C17" s="26">
@@ -7829,7 +7822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
       <c r="B18" s="23"/>
       <c r="C18" s="26">
@@ -7853,7 +7846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="24"/>
       <c r="B19" s="23"/>
       <c r="C19" s="26">
@@ -7877,7 +7870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
       <c r="B20" s="23"/>
       <c r="C20" s="26">
@@ -7901,7 +7894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="24"/>
       <c r="B21" s="23"/>
       <c r="C21" s="26">
@@ -7925,7 +7918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="24"/>
       <c r="B22" s="23"/>
       <c r="C22" s="26">
@@ -7949,7 +7942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="24"/>
       <c r="B23" s="23"/>
       <c r="C23" s="26">
@@ -7973,7 +7966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="24"/>
       <c r="B24" s="23"/>
       <c r="C24" s="26">
@@ -7997,7 +7990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="24"/>
       <c r="B25" s="23"/>
       <c r="C25" s="26">
@@ -8021,7 +8014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="24"/>
       <c r="B26" s="23"/>
       <c r="C26" s="26">
@@ -8045,7 +8038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="24"/>
       <c r="B27" s="23"/>
       <c r="C27" s="26">
@@ -8069,7 +8062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="24"/>
       <c r="B28" s="23"/>
       <c r="C28" s="26">
@@ -8093,7 +8086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="24"/>
       <c r="B29" s="23"/>
       <c r="C29" s="26">
@@ -8117,7 +8110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="24"/>
       <c r="B30" s="23"/>
       <c r="C30" s="26">
@@ -8141,7 +8134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="24"/>
       <c r="B31" s="23"/>
       <c r="C31" s="26">
@@ -8165,7 +8158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="24"/>
       <c r="B32" s="23"/>
       <c r="C32" s="26">
@@ -8189,7 +8182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="24"/>
       <c r="B33" s="23"/>
       <c r="C33" s="26">
@@ -8213,7 +8206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="17.25" thickBot="1">
+    <row r="34" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="24"/>
       <c r="B34" s="23"/>
       <c r="C34" s="27">
@@ -8237,8 +8230,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="17.25" thickBot="1"/>
-    <row r="38" spans="1:10" ht="21" thickTop="1" thickBot="1">
+    <row r="37" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:10" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="145" t="s">
         <v>43</v>
       </c>
@@ -8255,7 +8248,7 @@
       </c>
       <c r="H38" s="152"/>
     </row>
-    <row r="39" spans="1:10" ht="20.25" thickBot="1">
+    <row r="39" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="146"/>
       <c r="C39" s="124" t="s">
         <v>47</v>
@@ -8279,7 +8272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="20.25" thickBot="1">
+    <row r="40" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="146"/>
       <c r="C40" s="124" t="s">
         <v>49</v>
@@ -8301,7 +8294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="20.25" thickBot="1">
+    <row r="41" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="146"/>
       <c r="C41" s="124" t="s">
         <v>51</v>
@@ -8325,7 +8318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="20.25" thickBot="1">
+    <row r="42" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="147"/>
       <c r="C42" s="131" t="s">
         <v>53</v>
@@ -8347,7 +8340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="17.25" thickTop="1"/>
+    <row r="43" spans="1:10" ht="17.25" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="I1:J1"/>
@@ -8366,7 +8359,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
@@ -8376,7 +8369,7 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="45" customWidth="1"/>
     <col min="2" max="2" width="10.75" style="46" customWidth="1"/>
@@ -8390,7 +8383,7 @@
     <col min="10" max="10" width="10.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="141" t="s">
         <v>58</v>
       </c>
@@ -8406,7 +8399,7 @@
       </c>
       <c r="J1" s="75"/>
     </row>
-    <row r="2" spans="1:10" ht="57">
+    <row r="2" spans="1:10" ht="57" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -8438,7 +8431,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="42"/>
       <c r="B3" s="21"/>
       <c r="C3" s="36">
@@ -8452,7 +8445,7 @@
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="96"/>
       <c r="B4" s="97"/>
       <c r="C4" s="98">
@@ -8476,7 +8469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="96"/>
       <c r="B5" s="97"/>
       <c r="C5" s="98">
@@ -8500,7 +8493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="96"/>
       <c r="B6" s="97"/>
       <c r="C6" s="98">
@@ -8524,7 +8517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="96"/>
       <c r="B7" s="97"/>
       <c r="C7" s="98">
@@ -8548,7 +8541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="96"/>
       <c r="B8" s="97"/>
       <c r="C8" s="98">
@@ -8572,7 +8565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="96"/>
       <c r="B9" s="97"/>
       <c r="C9" s="98">
@@ -8596,7 +8589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="96"/>
       <c r="B10" s="97"/>
       <c r="C10" s="98">
@@ -8620,7 +8613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="96"/>
       <c r="B11" s="97"/>
       <c r="C11" s="98">
@@ -8644,7 +8637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="96"/>
       <c r="B12" s="97"/>
       <c r="C12" s="98">
@@ -8668,7 +8661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="96"/>
       <c r="B13" s="97"/>
       <c r="C13" s="98">
@@ -8692,7 +8685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="96"/>
       <c r="B14" s="97"/>
       <c r="C14" s="98">
@@ -8716,7 +8709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="96"/>
       <c r="B15" s="97"/>
       <c r="C15" s="98">
@@ -8740,7 +8733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="96"/>
       <c r="B16" s="97"/>
       <c r="C16" s="98">
@@ -8764,7 +8757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="96"/>
       <c r="B17" s="97"/>
       <c r="C17" s="98">
@@ -8788,7 +8781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="96"/>
       <c r="B18" s="97"/>
       <c r="C18" s="98">
@@ -8812,7 +8805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="96"/>
       <c r="B19" s="97"/>
       <c r="C19" s="98">
@@ -8836,7 +8829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="96"/>
       <c r="B20" s="97"/>
       <c r="C20" s="98">
@@ -8860,7 +8853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="96"/>
       <c r="B21" s="97"/>
       <c r="C21" s="98">
@@ -8884,7 +8877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="96"/>
       <c r="B22" s="97"/>
       <c r="C22" s="98">
@@ -8908,7 +8901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="96"/>
       <c r="B23" s="97"/>
       <c r="C23" s="98">
@@ -8932,7 +8925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="96"/>
       <c r="B24" s="97"/>
       <c r="C24" s="98">
@@ -8956,7 +8949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="96"/>
       <c r="B25" s="97"/>
       <c r="C25" s="98">
@@ -8980,7 +8973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="96"/>
       <c r="B26" s="97"/>
       <c r="C26" s="98">
@@ -9004,7 +8997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="96"/>
       <c r="B27" s="97"/>
       <c r="C27" s="98">
@@ -9028,7 +9021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="96"/>
       <c r="B28" s="97"/>
       <c r="C28" s="98">
@@ -9052,7 +9045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="96"/>
       <c r="B29" s="97"/>
       <c r="C29" s="98">
@@ -9076,7 +9069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="96"/>
       <c r="B30" s="97"/>
       <c r="C30" s="98">
@@ -9100,7 +9093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="96"/>
       <c r="B31" s="97"/>
       <c r="C31" s="98">
@@ -9124,7 +9117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="96"/>
       <c r="B32" s="97"/>
       <c r="C32" s="98">
@@ -9148,7 +9141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="96"/>
       <c r="B33" s="97"/>
       <c r="C33" s="98">
@@ -9172,7 +9165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="17.25" thickBot="1">
+    <row r="34" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="101"/>
       <c r="B34" s="102"/>
       <c r="C34" s="103">
@@ -9196,14 +9189,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E35" s="50"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E36" s="50"/>
     </row>
-    <row r="37" spans="1:10" ht="17.25" thickBot="1"/>
-    <row r="38" spans="1:10" ht="21" thickTop="1" thickBot="1">
+    <row r="37" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:10" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="188" t="s">
         <v>43</v>
       </c>
@@ -9220,7 +9213,7 @@
       </c>
       <c r="H38" s="195"/>
     </row>
-    <row r="39" spans="1:10" ht="20.25" thickBot="1">
+    <row r="39" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="189"/>
       <c r="C39" s="119" t="s">
         <v>47</v>
@@ -9244,7 +9237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="20.25" thickBot="1">
+    <row r="40" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="189"/>
       <c r="C40" s="119" t="s">
         <v>49</v>
@@ -9266,7 +9259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="20.25" thickBot="1">
+    <row r="41" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="189"/>
       <c r="C41" s="119" t="s">
         <v>51</v>
@@ -9290,7 +9283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="20.25" thickBot="1">
+    <row r="42" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B42" s="190"/>
       <c r="C42" s="121" t="s">
         <v>53</v>
@@ -9312,7 +9305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="17.25" thickTop="1"/>
+    <row r="43" spans="1:10" ht="17.25" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:G1"/>
@@ -9330,7 +9323,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
@@ -9340,7 +9333,7 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="45" customWidth="1"/>
     <col min="2" max="2" width="10.75" style="46" customWidth="1"/>
@@ -9354,7 +9347,7 @@
     <col min="10" max="10" width="10.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="196" t="s">
         <v>81</v>
       </c>
@@ -9370,7 +9363,7 @@
       </c>
       <c r="J1" s="79"/>
     </row>
-    <row r="2" spans="1:10" ht="63" customHeight="1">
+    <row r="2" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="80" t="s">
         <v>62</v>
       </c>
@@ -9402,7 +9395,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="42"/>
       <c r="B3" s="21"/>
       <c r="C3" s="36">
@@ -9416,7 +9409,7 @@
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="96"/>
       <c r="B4" s="97"/>
       <c r="C4" s="98">
@@ -9440,7 +9433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="96"/>
       <c r="B5" s="97"/>
       <c r="C5" s="98">
@@ -9464,7 +9457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="96"/>
       <c r="B6" s="97"/>
       <c r="C6" s="98">
@@ -9488,7 +9481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="96"/>
       <c r="B7" s="97"/>
       <c r="C7" s="98">
@@ -9512,7 +9505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="96"/>
       <c r="B8" s="97"/>
       <c r="C8" s="98">
@@ -9536,7 +9529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="96"/>
       <c r="B9" s="97"/>
       <c r="C9" s="98">
@@ -9560,7 +9553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="96"/>
       <c r="B10" s="97"/>
       <c r="C10" s="98">
@@ -9584,7 +9577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="96"/>
       <c r="B11" s="97"/>
       <c r="C11" s="98">
@@ -9608,7 +9601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="96"/>
       <c r="B12" s="97"/>
       <c r="C12" s="98">
@@ -9632,7 +9625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="96"/>
       <c r="B13" s="97"/>
       <c r="C13" s="98">
@@ -9656,7 +9649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="96"/>
       <c r="B14" s="97"/>
       <c r="C14" s="98">
@@ -9680,7 +9673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="96"/>
       <c r="B15" s="97"/>
       <c r="C15" s="98">
@@ -9704,7 +9697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="96"/>
       <c r="B16" s="97"/>
       <c r="C16" s="98">
@@ -9728,7 +9721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="96"/>
       <c r="B17" s="97"/>
       <c r="C17" s="98">
@@ -9752,7 +9745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="96"/>
       <c r="B18" s="97"/>
       <c r="C18" s="98">
@@ -9776,7 +9769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="96"/>
       <c r="B19" s="97"/>
       <c r="C19" s="98">
@@ -9800,7 +9793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="96"/>
       <c r="B20" s="97"/>
       <c r="C20" s="98">
@@ -9824,7 +9817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="96"/>
       <c r="B21" s="97"/>
       <c r="C21" s="98">
@@ -9848,7 +9841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="96"/>
       <c r="B22" s="97"/>
       <c r="C22" s="98">
@@ -9872,7 +9865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="96"/>
       <c r="B23" s="97"/>
       <c r="C23" s="98">
@@ -9896,7 +9889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="96"/>
       <c r="B24" s="97"/>
       <c r="C24" s="98">
@@ -9920,7 +9913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="96"/>
       <c r="B25" s="97"/>
       <c r="C25" s="98">
@@ -9944,7 +9937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="96"/>
       <c r="B26" s="97"/>
       <c r="C26" s="98">
@@ -9968,7 +9961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="96"/>
       <c r="B27" s="97"/>
       <c r="C27" s="98">
@@ -9992,7 +9985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="96"/>
       <c r="B28" s="97"/>
       <c r="C28" s="98">
@@ -10016,7 +10009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="96"/>
       <c r="B29" s="97"/>
       <c r="C29" s="98">
@@ -10040,7 +10033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="96"/>
       <c r="B30" s="97"/>
       <c r="C30" s="98">
@@ -10064,7 +10057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="96"/>
       <c r="B31" s="97"/>
       <c r="C31" s="98">
@@ -10088,7 +10081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="96"/>
       <c r="B32" s="97"/>
       <c r="C32" s="98">
@@ -10112,7 +10105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="96"/>
       <c r="B33" s="97"/>
       <c r="C33" s="98">
@@ -10136,7 +10129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="17.25" thickBot="1">
+    <row r="34" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="101"/>
       <c r="B34" s="102"/>
       <c r="C34" s="103">
@@ -10160,14 +10153,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E35" s="50"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E36" s="50"/>
     </row>
-    <row r="37" spans="1:10" ht="17.25" thickBot="1"/>
-    <row r="38" spans="1:10" ht="21" thickTop="1" thickBot="1">
+    <row r="37" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:10" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="200" t="s">
         <v>67</v>
       </c>
@@ -10184,7 +10177,7 @@
       </c>
       <c r="H38" s="207"/>
     </row>
-    <row r="39" spans="1:10" ht="20.25" thickBot="1">
+    <row r="39" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="201"/>
       <c r="C39" s="105" t="s">
         <v>71</v>
@@ -10208,7 +10201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="20.25" thickBot="1">
+    <row r="40" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="201"/>
       <c r="C40" s="105" t="s">
         <v>73</v>
@@ -10230,7 +10223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="20.25" thickBot="1">
+    <row r="41" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="201"/>
       <c r="C41" s="105" t="s">
         <v>75</v>
@@ -10254,7 +10247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="20.25" thickBot="1">
+    <row r="42" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B42" s="202"/>
       <c r="C42" s="113" t="s">
         <v>77</v>
@@ -10276,7 +10269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="17.25" thickTop="1"/>
+    <row r="43" spans="1:10" ht="17.25" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:G1"/>
@@ -10294,7 +10287,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -10304,7 +10297,7 @@
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="45" customWidth="1"/>
     <col min="2" max="2" width="10.75" style="46" customWidth="1"/>
@@ -10318,7 +10311,7 @@
     <col min="10" max="10" width="10.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="141" t="s">
         <v>90</v>
       </c>
@@ -10334,7 +10327,7 @@
       </c>
       <c r="J1" s="79"/>
     </row>
-    <row r="2" spans="1:10" ht="63" customHeight="1">
+    <row r="2" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="80" t="s">
         <v>62</v>
       </c>
@@ -10366,7 +10359,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="42"/>
       <c r="B3" s="21"/>
       <c r="C3" s="36">
@@ -10380,7 +10373,7 @@
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="96"/>
       <c r="B4" s="97"/>
       <c r="C4" s="98">
@@ -10404,7 +10397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="96"/>
       <c r="B5" s="97"/>
       <c r="C5" s="98">
@@ -10428,7 +10421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="96"/>
       <c r="B6" s="97"/>
       <c r="C6" s="98">
@@ -10452,7 +10445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="96"/>
       <c r="B7" s="97"/>
       <c r="C7" s="98">
@@ -10476,7 +10469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="96"/>
       <c r="B8" s="97"/>
       <c r="C8" s="98">
@@ -10500,7 +10493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="96"/>
       <c r="B9" s="97"/>
       <c r="C9" s="98">
@@ -10524,7 +10517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="96"/>
       <c r="B10" s="97"/>
       <c r="C10" s="98">
@@ -10548,7 +10541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="96"/>
       <c r="B11" s="97"/>
       <c r="C11" s="98">
@@ -10572,7 +10565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="96"/>
       <c r="B12" s="97"/>
       <c r="C12" s="98">
@@ -10596,7 +10589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="96"/>
       <c r="B13" s="97"/>
       <c r="C13" s="98">
@@ -10620,7 +10613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="96"/>
       <c r="B14" s="97"/>
       <c r="C14" s="98">
@@ -10644,7 +10637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="96"/>
       <c r="B15" s="97"/>
       <c r="C15" s="98">
@@ -10668,7 +10661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="96"/>
       <c r="B16" s="97"/>
       <c r="C16" s="98">
@@ -10692,7 +10685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="96"/>
       <c r="B17" s="97"/>
       <c r="C17" s="98">
@@ -10716,7 +10709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="96"/>
       <c r="B18" s="97"/>
       <c r="C18" s="98">
@@ -10740,7 +10733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="96"/>
       <c r="B19" s="97"/>
       <c r="C19" s="98">
@@ -10764,7 +10757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="96"/>
       <c r="B20" s="97"/>
       <c r="C20" s="98">
@@ -10788,7 +10781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="96"/>
       <c r="B21" s="97"/>
       <c r="C21" s="98">
@@ -10812,7 +10805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="96"/>
       <c r="B22" s="97"/>
       <c r="C22" s="98">
@@ -10836,7 +10829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="96"/>
       <c r="B23" s="97"/>
       <c r="C23" s="98">
@@ -10860,7 +10853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="96"/>
       <c r="B24" s="97"/>
       <c r="C24" s="98">
@@ -10884,7 +10877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="96"/>
       <c r="B25" s="97"/>
       <c r="C25" s="98">
@@ -10908,7 +10901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="96"/>
       <c r="B26" s="97"/>
       <c r="C26" s="98">
@@ -10932,7 +10925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="96"/>
       <c r="B27" s="97"/>
       <c r="C27" s="98">
@@ -10956,7 +10949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="96"/>
       <c r="B28" s="97"/>
       <c r="C28" s="98">
@@ -10980,7 +10973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="96"/>
       <c r="B29" s="97"/>
       <c r="C29" s="98">
@@ -11004,7 +10997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="96"/>
       <c r="B30" s="97"/>
       <c r="C30" s="98">
@@ -11028,7 +11021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="96"/>
       <c r="B31" s="97"/>
       <c r="C31" s="98">
@@ -11052,7 +11045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="96"/>
       <c r="B32" s="97"/>
       <c r="C32" s="98">
@@ -11076,7 +11069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="96"/>
       <c r="B33" s="97"/>
       <c r="C33" s="98">
@@ -11100,7 +11093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="17.25" thickBot="1">
+    <row r="34" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="101"/>
       <c r="B34" s="102"/>
       <c r="C34" s="103">
@@ -11124,14 +11117,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E35" s="50"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E36" s="50"/>
     </row>
-    <row r="37" spans="1:10" ht="17.25" thickBot="1"/>
-    <row r="38" spans="1:10" ht="21" thickTop="1" thickBot="1">
+    <row r="37" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:10" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="200" t="s">
         <v>67</v>
       </c>
@@ -11148,7 +11141,7 @@
       </c>
       <c r="H38" s="207"/>
     </row>
-    <row r="39" spans="1:10" ht="20.25" thickBot="1">
+    <row r="39" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="201"/>
       <c r="C39" s="105" t="s">
         <v>71</v>
@@ -11172,7 +11165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="20.25" thickBot="1">
+    <row r="40" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="201"/>
       <c r="C40" s="105" t="s">
         <v>73</v>
@@ -11194,7 +11187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="20.25" thickBot="1">
+    <row r="41" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="201"/>
       <c r="C41" s="105" t="s">
         <v>75</v>
@@ -11218,7 +11211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="20.25" thickBot="1">
+    <row r="42" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B42" s="202"/>
       <c r="C42" s="113" t="s">
         <v>77</v>
@@ -11240,7 +11233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="17.25" thickTop="1"/>
+    <row r="43" spans="1:10" ht="17.25" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:G1"/>
@@ -11258,7 +11251,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
@@ -11266,7 +11259,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.625" style="1" customWidth="1"/>
@@ -11289,7 +11282,7 @@
     <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16.5" customHeight="1">
+    <row r="1" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>58</v>
       </c>
@@ -11312,7 +11305,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15.2" customHeight="1">
+    <row r="2" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="153" t="s">
         <v>1</v>
       </c>
@@ -11339,7 +11332,7 @@
       </c>
       <c r="Q2" s="162"/>
     </row>
-    <row r="3" spans="1:20" ht="15.2" customHeight="1">
+    <row r="3" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="154"/>
       <c r="B3" s="164" t="s">
         <v>3</v>
@@ -11370,7 +11363,7 @@
       <c r="P3" s="161"/>
       <c r="Q3" s="163"/>
     </row>
-    <row r="4" spans="1:20" ht="15.2" customHeight="1">
+    <row r="4" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="154"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -11421,7 +11414,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15.2" customHeight="1">
+    <row r="5" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="86"/>
       <c r="B5" s="87"/>
       <c r="C5" s="87"/>
@@ -11449,7 +11442,7 @@
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
     </row>
-    <row r="6" spans="1:20" ht="15.2" customHeight="1">
+    <row r="6" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="86"/>
       <c r="B6" s="87"/>
       <c r="C6" s="87"/>
@@ -11477,7 +11470,7 @@
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
     </row>
-    <row r="7" spans="1:20" ht="15.2" customHeight="1">
+    <row r="7" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="86"/>
       <c r="B7" s="87"/>
       <c r="C7" s="87"/>
@@ -11505,7 +11498,7 @@
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
     </row>
-    <row r="8" spans="1:20" ht="15.2" customHeight="1">
+    <row r="8" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="86"/>
       <c r="B8" s="87"/>
       <c r="C8" s="87"/>
@@ -11533,7 +11526,7 @@
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
     </row>
-    <row r="9" spans="1:20" ht="15.2" customHeight="1">
+    <row r="9" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="89"/>
       <c r="B9" s="87"/>
       <c r="C9" s="87"/>
@@ -11561,7 +11554,7 @@
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
     </row>
-    <row r="10" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="10" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
       <c r="B10" s="87"/>
       <c r="C10" s="87"/>
@@ -11589,7 +11582,7 @@
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
     </row>
-    <row r="11" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="11" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="89"/>
       <c r="B11" s="87"/>
       <c r="C11" s="87"/>
@@ -11617,7 +11610,7 @@
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
     </row>
-    <row r="12" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="12" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="89"/>
       <c r="B12" s="87"/>
       <c r="C12" s="87"/>
@@ -11645,7 +11638,7 @@
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
     </row>
-    <row r="13" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="13" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="89"/>
       <c r="B13" s="87"/>
       <c r="C13" s="87"/>
@@ -11673,7 +11666,7 @@
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>
     </row>
-    <row r="14" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="14" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="89"/>
       <c r="B14" s="87"/>
       <c r="C14" s="87"/>
@@ -11701,7 +11694,7 @@
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
     </row>
-    <row r="15" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="15" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="89"/>
       <c r="B15" s="87"/>
       <c r="C15" s="87"/>
@@ -11729,7 +11722,7 @@
       <c r="S15" s="7"/>
       <c r="T15" s="7"/>
     </row>
-    <row r="16" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="16" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="89"/>
       <c r="B16" s="87"/>
       <c r="C16" s="87"/>
@@ -11757,7 +11750,7 @@
       <c r="S16" s="7"/>
       <c r="T16" s="7"/>
     </row>
-    <row r="17" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="17" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="90" t="s">
         <v>79</v>
       </c>
@@ -11829,7 +11822,7 @@
       <c r="S17" s="11"/>
       <c r="T17" s="11"/>
     </row>
-    <row r="18" spans="1:20" s="13" customFormat="1">
+    <row r="18" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="92" t="s">
         <v>12</v>
       </c>
@@ -11898,7 +11891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>13</v>
       </c>
@@ -11925,7 +11918,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
@@ -11935,7 +11928,7 @@
       <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.625" style="1" customWidth="1"/>
@@ -11958,7 +11951,7 @@
     <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16.5" customHeight="1">
+    <row r="1" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>85</v>
       </c>
@@ -11981,7 +11974,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15.2" customHeight="1">
+    <row r="2" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="153" t="s">
         <v>1</v>
       </c>
@@ -12008,7 +12001,7 @@
       </c>
       <c r="Q2" s="162"/>
     </row>
-    <row r="3" spans="1:20" ht="15.2" customHeight="1">
+    <row r="3" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="154"/>
       <c r="B3" s="164" t="s">
         <v>3</v>
@@ -12039,7 +12032,7 @@
       <c r="P3" s="161"/>
       <c r="Q3" s="163"/>
     </row>
-    <row r="4" spans="1:20" ht="15.2" customHeight="1">
+    <row r="4" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="154"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -12090,7 +12083,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15.2" customHeight="1">
+    <row r="5" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="86"/>
       <c r="B5" s="87"/>
       <c r="C5" s="87"/>
@@ -12118,7 +12111,7 @@
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
     </row>
-    <row r="6" spans="1:20" ht="15.2" customHeight="1">
+    <row r="6" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="86"/>
       <c r="B6" s="87"/>
       <c r="C6" s="87"/>
@@ -12146,7 +12139,7 @@
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
     </row>
-    <row r="7" spans="1:20" ht="15.2" customHeight="1">
+    <row r="7" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="86"/>
       <c r="B7" s="87"/>
       <c r="C7" s="87"/>
@@ -12174,7 +12167,7 @@
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
     </row>
-    <row r="8" spans="1:20" ht="15.2" customHeight="1">
+    <row r="8" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="86"/>
       <c r="B8" s="87"/>
       <c r="C8" s="87"/>
@@ -12202,7 +12195,7 @@
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
     </row>
-    <row r="9" spans="1:20" ht="15.2" customHeight="1">
+    <row r="9" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="89"/>
       <c r="B9" s="87"/>
       <c r="C9" s="87"/>
@@ -12230,7 +12223,7 @@
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
     </row>
-    <row r="10" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="10" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
       <c r="B10" s="87"/>
       <c r="C10" s="87"/>
@@ -12258,7 +12251,7 @@
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
     </row>
-    <row r="11" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="11" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="89"/>
       <c r="B11" s="87"/>
       <c r="C11" s="87"/>
@@ -12286,7 +12279,7 @@
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
     </row>
-    <row r="12" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="12" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="89"/>
       <c r="B12" s="87"/>
       <c r="C12" s="87"/>
@@ -12314,7 +12307,7 @@
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
     </row>
-    <row r="13" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="13" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="89"/>
       <c r="B13" s="87"/>
       <c r="C13" s="87"/>
@@ -12342,7 +12335,7 @@
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>
     </row>
-    <row r="14" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="14" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="89"/>
       <c r="B14" s="87"/>
       <c r="C14" s="87"/>
@@ -12370,7 +12363,7 @@
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
     </row>
-    <row r="15" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="15" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="89"/>
       <c r="B15" s="87"/>
       <c r="C15" s="87"/>
@@ -12398,7 +12391,7 @@
       <c r="S15" s="7"/>
       <c r="T15" s="7"/>
     </row>
-    <row r="16" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="16" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="89"/>
       <c r="B16" s="87"/>
       <c r="C16" s="87"/>
@@ -12426,7 +12419,7 @@
       <c r="S16" s="7"/>
       <c r="T16" s="7"/>
     </row>
-    <row r="17" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="17" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="90" t="s">
         <v>79</v>
       </c>
@@ -12498,7 +12491,7 @@
       <c r="S17" s="11"/>
       <c r="T17" s="11"/>
     </row>
-    <row r="18" spans="1:20" s="13" customFormat="1">
+    <row r="18" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="92" t="s">
         <v>12</v>
       </c>
@@ -12567,7 +12560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>13</v>
       </c>
@@ -12594,7 +12587,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -12604,7 +12597,7 @@
       <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.625" style="1" customWidth="1"/>
@@ -12627,7 +12620,7 @@
     <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16.5" customHeight="1">
+    <row r="1" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>90</v>
       </c>
@@ -12650,7 +12643,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15.2" customHeight="1">
+    <row r="2" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="153" t="s">
         <v>1</v>
       </c>
@@ -12677,7 +12670,7 @@
       </c>
       <c r="Q2" s="162"/>
     </row>
-    <row r="3" spans="1:20" ht="15.2" customHeight="1">
+    <row r="3" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="154"/>
       <c r="B3" s="164" t="s">
         <v>3</v>
@@ -12708,7 +12701,7 @@
       <c r="P3" s="161"/>
       <c r="Q3" s="163"/>
     </row>
-    <row r="4" spans="1:20" ht="15.2" customHeight="1">
+    <row r="4" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="154"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -12759,7 +12752,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15.2" customHeight="1">
+    <row r="5" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="86"/>
       <c r="B5" s="87"/>
       <c r="C5" s="87"/>
@@ -12787,7 +12780,7 @@
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
     </row>
-    <row r="6" spans="1:20" ht="15.2" customHeight="1">
+    <row r="6" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="86"/>
       <c r="B6" s="87"/>
       <c r="C6" s="87"/>
@@ -12815,7 +12808,7 @@
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
     </row>
-    <row r="7" spans="1:20" ht="15.2" customHeight="1">
+    <row r="7" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="86"/>
       <c r="B7" s="87"/>
       <c r="C7" s="87"/>
@@ -12843,7 +12836,7 @@
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
     </row>
-    <row r="8" spans="1:20" ht="15.2" customHeight="1">
+    <row r="8" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="86"/>
       <c r="B8" s="87"/>
       <c r="C8" s="87"/>
@@ -12871,7 +12864,7 @@
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
     </row>
-    <row r="9" spans="1:20" ht="15.2" customHeight="1">
+    <row r="9" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="89"/>
       <c r="B9" s="87"/>
       <c r="C9" s="87"/>
@@ -12899,7 +12892,7 @@
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
     </row>
-    <row r="10" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="10" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
       <c r="B10" s="87"/>
       <c r="C10" s="87"/>
@@ -12927,7 +12920,7 @@
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
     </row>
-    <row r="11" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="11" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="89"/>
       <c r="B11" s="87"/>
       <c r="C11" s="87"/>
@@ -12955,7 +12948,7 @@
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
     </row>
-    <row r="12" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="12" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="89"/>
       <c r="B12" s="87"/>
       <c r="C12" s="87"/>
@@ -12983,7 +12976,7 @@
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
     </row>
-    <row r="13" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="13" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="89"/>
       <c r="B13" s="87"/>
       <c r="C13" s="87"/>
@@ -13011,7 +13004,7 @@
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>
     </row>
-    <row r="14" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="14" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="89"/>
       <c r="B14" s="87"/>
       <c r="C14" s="87"/>
@@ -13039,7 +13032,7 @@
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
     </row>
-    <row r="15" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="15" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="89"/>
       <c r="B15" s="87"/>
       <c r="C15" s="87"/>
@@ -13067,7 +13060,7 @@
       <c r="S15" s="7"/>
       <c r="T15" s="7"/>
     </row>
-    <row r="16" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="16" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="89"/>
       <c r="B16" s="87"/>
       <c r="C16" s="87"/>
@@ -13095,7 +13088,7 @@
       <c r="S16" s="7"/>
       <c r="T16" s="7"/>
     </row>
-    <row r="17" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="17" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="90" t="s">
         <v>79</v>
       </c>
@@ -13167,7 +13160,7 @@
       <c r="S17" s="11"/>
       <c r="T17" s="11"/>
     </row>
-    <row r="18" spans="1:20" s="13" customFormat="1">
+    <row r="18" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="92" t="s">
         <v>12</v>
       </c>
@@ -13236,7 +13229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>13</v>
       </c>
@@ -13263,14 +13256,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13280,14 +13273,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13297,7 +13290,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
@@ -13305,7 +13298,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.625" style="1" customWidth="1"/>
@@ -13328,7 +13321,7 @@
     <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16.5" customHeight="1">
+    <row r="1" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="40" t="s">
         <v>37</v>
       </c>
@@ -13351,7 +13344,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15.2" customHeight="1">
+    <row r="2" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="153" t="s">
         <v>1</v>
       </c>
@@ -13378,7 +13371,7 @@
       </c>
       <c r="Q2" s="162"/>
     </row>
-    <row r="3" spans="1:20" ht="15.2" customHeight="1">
+    <row r="3" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="154"/>
       <c r="B3" s="164" t="s">
         <v>3</v>
@@ -13409,7 +13402,7 @@
       <c r="P3" s="161"/>
       <c r="Q3" s="163"/>
     </row>
-    <row r="4" spans="1:20" ht="15.2" customHeight="1">
+    <row r="4" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="154"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -13460,7 +13453,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15.2" customHeight="1">
+    <row r="5" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="86"/>
       <c r="B5" s="87"/>
       <c r="C5" s="87"/>
@@ -13488,7 +13481,7 @@
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
     </row>
-    <row r="6" spans="1:20" ht="15.2" customHeight="1">
+    <row r="6" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="86"/>
       <c r="B6" s="87"/>
       <c r="C6" s="87"/>
@@ -13516,7 +13509,7 @@
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
     </row>
-    <row r="7" spans="1:20" ht="15.2" customHeight="1">
+    <row r="7" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="86"/>
       <c r="B7" s="87"/>
       <c r="C7" s="87"/>
@@ -13544,7 +13537,7 @@
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
     </row>
-    <row r="8" spans="1:20" ht="15.2" customHeight="1">
+    <row r="8" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="86"/>
       <c r="B8" s="87"/>
       <c r="C8" s="87"/>
@@ -13572,7 +13565,7 @@
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
     </row>
-    <row r="9" spans="1:20" ht="15.2" customHeight="1">
+    <row r="9" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="89"/>
       <c r="B9" s="87"/>
       <c r="C9" s="87"/>
@@ -13600,7 +13593,7 @@
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
     </row>
-    <row r="10" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="10" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="89"/>
       <c r="B10" s="87"/>
       <c r="C10" s="87"/>
@@ -13628,7 +13621,7 @@
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
     </row>
-    <row r="11" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="11" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="89"/>
       <c r="B11" s="87"/>
       <c r="C11" s="87"/>
@@ -13656,7 +13649,7 @@
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
     </row>
-    <row r="12" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="12" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="89"/>
       <c r="B12" s="87"/>
       <c r="C12" s="87"/>
@@ -13684,7 +13677,7 @@
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
     </row>
-    <row r="13" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="13" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="89"/>
       <c r="B13" s="87"/>
       <c r="C13" s="87"/>
@@ -13712,7 +13705,7 @@
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>
     </row>
-    <row r="14" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="14" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="89"/>
       <c r="B14" s="87"/>
       <c r="C14" s="87"/>
@@ -13740,7 +13733,7 @@
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
     </row>
-    <row r="15" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="15" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="89"/>
       <c r="B15" s="87"/>
       <c r="C15" s="87"/>
@@ -13768,7 +13761,7 @@
       <c r="S15" s="7"/>
       <c r="T15" s="7"/>
     </row>
-    <row r="16" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="16" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="89"/>
       <c r="B16" s="87"/>
       <c r="C16" s="87"/>
@@ -13796,7 +13789,7 @@
       <c r="S16" s="7"/>
       <c r="T16" s="7"/>
     </row>
-    <row r="17" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="17" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="90" t="s">
         <v>79</v>
       </c>
@@ -13868,7 +13861,7 @@
       <c r="S17" s="11"/>
       <c r="T17" s="11"/>
     </row>
-    <row r="18" spans="1:20" s="13" customFormat="1">
+    <row r="18" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="92" t="s">
         <v>12</v>
       </c>
@@ -13937,7 +13930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>13</v>
       </c>
@@ -13964,7 +13957,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -13974,14 +13967,14 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.625" style="30" customWidth="1"/>
     <col min="2" max="11" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" hidden="1"/>
-    <row r="2" spans="1:11" ht="18" customHeight="1">
+    <row r="1" spans="1:11" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="173" t="s">
         <v>0</v>
       </c>
@@ -13998,7 +13991,7 @@
       <c r="J2" s="177"/>
       <c r="K2" s="178"/>
     </row>
-    <row r="3" spans="1:11" ht="18" customHeight="1">
+    <row r="3" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="174"/>
       <c r="B3" s="179" t="s">
         <v>24</v>
@@ -14021,7 +14014,7 @@
       <c r="J3" s="182"/>
       <c r="K3" s="181"/>
     </row>
-    <row r="4" spans="1:11" ht="18" customHeight="1">
+    <row r="4" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="175"/>
       <c r="B4" s="175"/>
       <c r="C4" s="175"/>
@@ -14050,7 +14043,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="18" customHeight="1">
+    <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33"/>
       <c r="B5" s="31"/>
       <c r="C5" s="31"/>
@@ -14063,7 +14056,7 @@
       <c r="J5" s="32"/>
       <c r="K5" s="32"/>
     </row>
-    <row r="6" spans="1:11" ht="18" customHeight="1">
+    <row r="6" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="33"/>
       <c r="B6" s="31"/>
       <c r="C6" s="31"/>
@@ -14076,7 +14069,7 @@
       <c r="J6" s="32"/>
       <c r="K6" s="32"/>
     </row>
-    <row r="7" spans="1:11" ht="18" customHeight="1">
+    <row r="7" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="33"/>
       <c r="B7" s="31"/>
       <c r="C7" s="31"/>
@@ -14089,7 +14082,7 @@
       <c r="J7" s="32"/>
       <c r="K7" s="32"/>
     </row>
-    <row r="8" spans="1:11" ht="18" customHeight="1">
+    <row r="8" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="33"/>
       <c r="B8" s="31"/>
       <c r="C8" s="31"/>
@@ -14102,7 +14095,7 @@
       <c r="J8" s="32"/>
       <c r="K8" s="32"/>
     </row>
-    <row r="9" spans="1:11" ht="18" customHeight="1">
+    <row r="9" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="33"/>
       <c r="B9" s="31"/>
       <c r="C9" s="31"/>
@@ -14115,7 +14108,7 @@
       <c r="J9" s="32"/>
       <c r="K9" s="32"/>
     </row>
-    <row r="10" spans="1:11" ht="18" customHeight="1">
+    <row r="10" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="33"/>
       <c r="B10" s="31"/>
       <c r="C10" s="31"/>
@@ -14128,7 +14121,7 @@
       <c r="J10" s="32"/>
       <c r="K10" s="32"/>
     </row>
-    <row r="11" spans="1:11" ht="18" customHeight="1">
+    <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="33"/>
       <c r="B11" s="31"/>
       <c r="C11" s="31"/>
@@ -14141,7 +14134,7 @@
       <c r="J11" s="32"/>
       <c r="K11" s="32"/>
     </row>
-    <row r="12" spans="1:11" ht="18" customHeight="1">
+    <row r="12" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="33"/>
       <c r="B12" s="31"/>
       <c r="C12" s="31"/>
@@ -14154,7 +14147,7 @@
       <c r="J12" s="32"/>
       <c r="K12" s="32"/>
     </row>
-    <row r="13" spans="1:11" ht="18" customHeight="1">
+    <row r="13" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33"/>
       <c r="B13" s="31"/>
       <c r="C13" s="31"/>
@@ -14167,7 +14160,7 @@
       <c r="J13" s="32"/>
       <c r="K13" s="32"/>
     </row>
-    <row r="14" spans="1:11" ht="18" customHeight="1">
+    <row r="14" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33"/>
       <c r="B14" s="31"/>
       <c r="C14" s="31"/>
@@ -14180,7 +14173,7 @@
       <c r="J14" s="32"/>
       <c r="K14" s="32"/>
     </row>
-    <row r="15" spans="1:11" ht="18" customHeight="1">
+    <row r="15" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
       <c r="B15" s="31"/>
       <c r="C15" s="31"/>
@@ -14193,7 +14186,7 @@
       <c r="J15" s="32"/>
       <c r="K15" s="32"/>
     </row>
-    <row r="16" spans="1:11" ht="18" customHeight="1">
+    <row r="16" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33"/>
       <c r="B16" s="31"/>
       <c r="C16" s="31"/>
@@ -14206,7 +14199,7 @@
       <c r="J16" s="32"/>
       <c r="K16" s="32"/>
     </row>
-    <row r="17" spans="1:11" ht="18" customHeight="1">
+    <row r="17" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="33"/>
       <c r="B17" s="31"/>
       <c r="C17" s="31"/>
@@ -14219,7 +14212,7 @@
       <c r="J17" s="32"/>
       <c r="K17" s="32"/>
     </row>
-    <row r="18" spans="1:11" ht="18" customHeight="1">
+    <row r="18" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="33"/>
       <c r="B18" s="31"/>
       <c r="C18" s="31"/>
@@ -14232,7 +14225,7 @@
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
     </row>
-    <row r="19" spans="1:11" ht="18" customHeight="1">
+    <row r="19" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="33"/>
       <c r="B19" s="31"/>
       <c r="C19" s="31"/>
@@ -14245,7 +14238,7 @@
       <c r="J19" s="32"/>
       <c r="K19" s="32"/>
     </row>
-    <row r="20" spans="1:11" ht="18" customHeight="1">
+    <row r="20" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="33"/>
       <c r="B20" s="31"/>
       <c r="C20" s="31"/>
@@ -14258,7 +14251,7 @@
       <c r="J20" s="32"/>
       <c r="K20" s="32"/>
     </row>
-    <row r="21" spans="1:11" ht="18" customHeight="1">
+    <row r="21" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="33"/>
       <c r="B21" s="31"/>
       <c r="C21" s="31"/>
@@ -14271,7 +14264,7 @@
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
     </row>
-    <row r="22" spans="1:11" ht="18" customHeight="1">
+    <row r="22" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="33"/>
       <c r="B22" s="31"/>
       <c r="C22" s="31"/>
@@ -14284,7 +14277,7 @@
       <c r="J22" s="32"/>
       <c r="K22" s="32"/>
     </row>
-    <row r="23" spans="1:11" ht="18" customHeight="1">
+    <row r="23" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="33"/>
       <c r="B23" s="31"/>
       <c r="C23" s="31"/>
@@ -14297,7 +14290,7 @@
       <c r="J23" s="32"/>
       <c r="K23" s="32"/>
     </row>
-    <row r="24" spans="1:11" ht="18" customHeight="1">
+    <row r="24" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="33"/>
       <c r="B24" s="31"/>
       <c r="C24" s="31"/>
@@ -14310,7 +14303,7 @@
       <c r="J24" s="32"/>
       <c r="K24" s="32"/>
     </row>
-    <row r="25" spans="1:11" ht="18" customHeight="1">
+    <row r="25" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="33"/>
       <c r="B25" s="31"/>
       <c r="C25" s="31"/>
@@ -14323,7 +14316,7 @@
       <c r="J25" s="32"/>
       <c r="K25" s="32"/>
     </row>
-    <row r="26" spans="1:11" ht="18" customHeight="1">
+    <row r="26" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="33"/>
       <c r="B26" s="31"/>
       <c r="C26" s="31"/>
@@ -14336,7 +14329,7 @@
       <c r="J26" s="32"/>
       <c r="K26" s="32"/>
     </row>
-    <row r="27" spans="1:11" ht="18" customHeight="1">
+    <row r="27" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="33"/>
       <c r="B27" s="31"/>
       <c r="C27" s="31"/>
@@ -14349,7 +14342,7 @@
       <c r="J27" s="32"/>
       <c r="K27" s="32"/>
     </row>
-    <row r="28" spans="1:11" ht="18" customHeight="1">
+    <row r="28" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="33"/>
       <c r="B28" s="31"/>
       <c r="C28" s="31"/>
@@ -14362,7 +14355,7 @@
       <c r="J28" s="32"/>
       <c r="K28" s="32"/>
     </row>
-    <row r="29" spans="1:11" ht="18" customHeight="1">
+    <row r="29" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="33"/>
       <c r="B29" s="31"/>
       <c r="C29" s="31"/>
@@ -14375,7 +14368,7 @@
       <c r="J29" s="32"/>
       <c r="K29" s="32"/>
     </row>
-    <row r="30" spans="1:11" ht="18" customHeight="1">
+    <row r="30" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="33"/>
       <c r="B30" s="31"/>
       <c r="C30" s="31"/>
@@ -14388,7 +14381,7 @@
       <c r="J30" s="32"/>
       <c r="K30" s="32"/>
     </row>
-    <row r="31" spans="1:11" ht="18" customHeight="1">
+    <row r="31" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="33"/>
       <c r="B31" s="31"/>
       <c r="C31" s="31"/>
@@ -14401,7 +14394,7 @@
       <c r="J31" s="32"/>
       <c r="K31" s="32"/>
     </row>
-    <row r="32" spans="1:11" ht="18" customHeight="1">
+    <row r="32" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="33"/>
       <c r="B32" s="31"/>
       <c r="C32" s="31"/>
@@ -14414,7 +14407,7 @@
       <c r="J32" s="32"/>
       <c r="K32" s="32"/>
     </row>
-    <row r="33" spans="1:11" ht="18" customHeight="1">
+    <row r="33" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="33"/>
       <c r="B33" s="31"/>
       <c r="C33" s="31"/>
@@ -14427,7 +14420,7 @@
       <c r="J33" s="32"/>
       <c r="K33" s="32"/>
     </row>
-    <row r="34" spans="1:11" ht="18" customHeight="1">
+    <row r="34" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="33"/>
       <c r="B34" s="31"/>
       <c r="C34" s="31"/>
@@ -14440,7 +14433,7 @@
       <c r="J34" s="32"/>
       <c r="K34" s="32"/>
     </row>
-    <row r="35" spans="1:11" ht="18" customHeight="1">
+    <row r="35" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="33"/>
       <c r="B35" s="31"/>
       <c r="C35" s="31"/>
@@ -14453,7 +14446,7 @@
       <c r="J35" s="32"/>
       <c r="K35" s="32"/>
     </row>
-    <row r="36" spans="1:11" ht="18" customHeight="1">
+    <row r="36" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="170" t="s">
         <v>32</v>
       </c>
@@ -14468,7 +14461,7 @@
       <c r="J36" s="171"/>
       <c r="K36" s="171"/>
     </row>
-    <row r="37" spans="1:11" ht="18" customHeight="1">
+    <row r="37" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="172"/>
       <c r="B37" s="172"/>
       <c r="C37" s="172"/>
@@ -14499,17 +14492,17 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="140" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" style="45" customWidth="1"/>
     <col min="2" max="2" width="12" style="46" customWidth="1"/>
@@ -14520,7 +14513,7 @@
     <col min="8" max="8" width="10.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="141" t="s">
         <v>41</v>
       </c>
@@ -14536,7 +14529,7 @@
       </c>
       <c r="J1" s="75"/>
     </row>
-    <row r="2" spans="1:10" ht="55.5">
+    <row r="2" spans="1:10" ht="55.5" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
@@ -14568,7 +14561,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="42"/>
       <c r="B3" s="21"/>
       <c r="C3" s="36">
@@ -14582,7 +14575,7 @@
       <c r="I3" s="21"/>
       <c r="J3" s="21"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="42"/>
       <c r="B4" s="21"/>
       <c r="C4" s="136">
@@ -14606,7 +14599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="42"/>
       <c r="B5" s="21"/>
       <c r="C5" s="136">
@@ -14630,7 +14623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="42"/>
       <c r="B6" s="21"/>
       <c r="C6" s="136">
@@ -14654,7 +14647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="42"/>
       <c r="B7" s="21"/>
       <c r="C7" s="136">
@@ -14678,7 +14671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="42"/>
       <c r="B8" s="21"/>
       <c r="C8" s="136">
@@ -14702,7 +14695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="42"/>
       <c r="B9" s="21"/>
       <c r="C9" s="136">
@@ -14726,7 +14719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
       <c r="B10" s="21"/>
       <c r="C10" s="136">
@@ -14750,7 +14743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="42"/>
       <c r="B11" s="21"/>
       <c r="C11" s="136">
@@ -14774,7 +14767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="42"/>
       <c r="B12" s="21"/>
       <c r="C12" s="136">
@@ -14798,7 +14791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="42"/>
       <c r="B13" s="21"/>
       <c r="C13" s="136">
@@ -14822,7 +14815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="42"/>
       <c r="B14" s="21"/>
       <c r="C14" s="136">
@@ -14846,7 +14839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="42"/>
       <c r="B15" s="21"/>
       <c r="C15" s="136">
@@ -14870,7 +14863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="42"/>
       <c r="B16" s="21"/>
       <c r="C16" s="136">
@@ -14894,7 +14887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="42"/>
       <c r="B17" s="21"/>
       <c r="C17" s="136">
@@ -14918,7 +14911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="42"/>
       <c r="B18" s="21"/>
       <c r="C18" s="136">
@@ -14942,7 +14935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="42"/>
       <c r="B19" s="21"/>
       <c r="C19" s="136">
@@ -14966,7 +14959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="42"/>
       <c r="B20" s="21"/>
       <c r="C20" s="136">
@@ -14990,7 +14983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="42"/>
       <c r="B21" s="21"/>
       <c r="C21" s="136">
@@ -15014,7 +15007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="42"/>
       <c r="B22" s="21"/>
       <c r="C22" s="136">
@@ -15038,7 +15031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="42"/>
       <c r="B23" s="21"/>
       <c r="C23" s="136">
@@ -15062,7 +15055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="42"/>
       <c r="B24" s="21"/>
       <c r="C24" s="136">
@@ -15086,7 +15079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="42"/>
       <c r="B25" s="21"/>
       <c r="C25" s="136">
@@ -15110,7 +15103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="42"/>
       <c r="B26" s="21"/>
       <c r="C26" s="136">
@@ -15134,7 +15127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="42"/>
       <c r="B27" s="21"/>
       <c r="C27" s="136">
@@ -15158,7 +15151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="42"/>
       <c r="B28" s="21"/>
       <c r="C28" s="136">
@@ -15182,7 +15175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="42"/>
       <c r="B29" s="21"/>
       <c r="C29" s="136">
@@ -15206,7 +15199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="42"/>
       <c r="B30" s="21"/>
       <c r="C30" s="136">
@@ -15230,7 +15223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="42"/>
       <c r="B31" s="21"/>
       <c r="C31" s="136">
@@ -15254,7 +15247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="42"/>
       <c r="B32" s="21"/>
       <c r="C32" s="136">
@@ -15278,7 +15271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="42"/>
       <c r="B33" s="21"/>
       <c r="C33" s="136">
@@ -15302,7 +15295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="17.25" thickBot="1">
+    <row r="34" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="43"/>
       <c r="B34" s="44"/>
       <c r="C34" s="137">
@@ -15326,14 +15319,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E35" s="50"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E36" s="50"/>
     </row>
-    <row r="37" spans="1:10" ht="17.25" thickBot="1"/>
-    <row r="38" spans="1:10" ht="21" thickTop="1" thickBot="1">
+    <row r="37" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:10" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="145" t="s">
         <v>43</v>
       </c>
@@ -15350,7 +15343,7 @@
       </c>
       <c r="H38" s="187"/>
     </row>
-    <row r="39" spans="1:10" ht="20.25" thickBot="1">
+    <row r="39" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="146"/>
       <c r="C39" s="53" t="s">
         <v>47</v>
@@ -15374,7 +15367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="20.25" thickBot="1">
+    <row r="40" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B40" s="146"/>
       <c r="C40" s="53" t="s">
         <v>49</v>
@@ -15396,7 +15389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="20.25" thickBot="1">
+    <row r="41" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="146"/>
       <c r="C41" s="53" t="s">
         <v>51</v>
@@ -15420,7 +15413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="20.25" thickBot="1">
+    <row r="42" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B42" s="147"/>
       <c r="C42" s="55" t="s">
         <v>53</v>
@@ -15442,7 +15435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="17.25" thickTop="1"/>
+    <row r="43" spans="1:10" ht="17.25" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:G1"/>
@@ -15460,14 +15453,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15477,14 +15470,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15494,12 +15487,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.625" style="1" customWidth="1"/>
@@ -15522,7 +15515,7 @@
     <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="16.5" customHeight="1">
+    <row r="1" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
         <v>36</v>
       </c>
@@ -15545,7 +15538,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15.2" customHeight="1">
+    <row r="2" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="153" t="s">
         <v>1</v>
       </c>
@@ -15572,7 +15565,7 @@
       </c>
       <c r="Q2" s="162"/>
     </row>
-    <row r="3" spans="1:20" ht="15.2" customHeight="1">
+    <row r="3" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="154"/>
       <c r="B3" s="164" t="s">
         <v>3</v>
@@ -15603,7 +15596,7 @@
       <c r="P3" s="161"/>
       <c r="Q3" s="163"/>
     </row>
-    <row r="4" spans="1:20" ht="15.2" customHeight="1">
+    <row r="4" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="154"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -15654,7 +15647,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="15.2" customHeight="1">
+    <row r="5" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="38"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -15682,7 +15675,7 @@
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
     </row>
-    <row r="6" spans="1:20" ht="15.2" customHeight="1">
+    <row r="6" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="38"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -15710,7 +15703,7 @@
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
     </row>
-    <row r="7" spans="1:20" ht="15.2" customHeight="1">
+    <row r="7" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="38"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -15738,7 +15731,7 @@
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
     </row>
-    <row r="8" spans="1:20" ht="15.2" customHeight="1">
+    <row r="8" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="38"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -15766,7 +15759,7 @@
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
     </row>
-    <row r="9" spans="1:20" ht="15.2" customHeight="1">
+    <row r="9" spans="1:20" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -15794,7 +15787,7 @@
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
     </row>
-    <row r="10" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="10" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="39"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -15822,7 +15815,7 @@
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
     </row>
-    <row r="11" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="11" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="39"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -15850,7 +15843,7 @@
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
     </row>
-    <row r="12" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="12" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="39"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -15878,7 +15871,7 @@
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
     </row>
-    <row r="13" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="13" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="39"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -15906,7 +15899,7 @@
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>
     </row>
-    <row r="14" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="14" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="39"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -15934,7 +15927,7 @@
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
     </row>
-    <row r="15" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="15" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="39"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -15962,7 +15955,7 @@
       <c r="S15" s="7"/>
       <c r="T15" s="7"/>
     </row>
-    <row r="16" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="16" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="39"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -15990,7 +15983,7 @@
       <c r="S16" s="7"/>
       <c r="T16" s="7"/>
     </row>
-    <row r="17" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1">
+    <row r="17" spans="1:20" s="8" customFormat="1" ht="15.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="85" t="s">
         <v>79</v>
       </c>
@@ -16062,7 +16055,7 @@
       <c r="S17" s="11"/>
       <c r="T17" s="11"/>
     </row>
-    <row r="18" spans="1:20" s="13" customFormat="1">
+    <row r="18" spans="1:20" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>12</v>
       </c>
@@ -16131,7 +16124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C21" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>